<commit_message>
update sensitivity handling and exp handling
</commit_message>
<xml_diff>
--- a/exp test.xlsx
+++ b/exp test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD87E199-F131-4B59-9A4B-64C16FB69243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E8D9DE-F7EA-4024-87E2-38B767583936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <author>Michael Young</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C8E28BEC-C1EE-4F3D-870D-9B724D3A3FA6}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Michael Young:</t>
         </r>
@@ -55,14 +55,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-this is the sen variable name - it is needed</t>
+Optional
+- Needed for pas</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{E327CCF7-BE60-470E-9304-A04607C4A9EF}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
       <text>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Michael Young:</t>
         </r>
@@ -79,11 +80,12 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-if necessary you can include a slice here, note-don't include the brackets.
-Slice is also non inclusive</t>
+Optional
+- needed for arrays
+- can handel complex slicing I think</t>
         </r>
       </text>
     </comment>
@@ -92,15 +94,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>sam_germ_l</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>0:1</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>germ_l</t>
+  </si>
+  <si>
+    <t>Dict</t>
+  </si>
+  <si>
+    <t>Key1</t>
+  </si>
+  <si>
+    <t>Key2</t>
+  </si>
+  <si>
+    <t>slice</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -119,22 +139,28 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -158,6 +184,13 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,35 +505,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="166.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6">
         <v>20</v>
       </c>
     </row>

</xml_diff>